<commit_message>
complete inv customer maintain
</commit_message>
<xml_diff>
--- a/mars/static/uploads/customer_list_template.xlsx
+++ b/mars/static/uploads/customer_list_template.xlsx
@@ -436,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>